<commit_message>
Adding more info to the excel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="126">
   <si>
     <t>Brand</t>
   </si>
@@ -378,16 +378,25 @@
     <t>https://www.flipkart.com/wings-hawk-65ms-low-latency-bluetooth-gaming-headset/p/itm033aa1785a71a?pid=ACCGAEEWJZCUZHMC&amp;lid=LSTACCGAEEWJZCUZHMCS1CL5G&amp;marketplace=FLIPKART&amp;q=gaming+earbuds&amp;store=0pm%2Ffcn&amp;srno=s_6_233&amp;otracker=search&amp;otracker1=search&amp;fm=Search&amp;iid=6571dfa9-7532-4f7e-aa2b-d83fe797a026.ACCGAEEWJZCUZHMC.SEARCH&amp;ppt=sp&amp;ppn=sp&amp;qH=fee236a6279bb73e</t>
   </si>
   <si>
+    <t>Rev - 9/1</t>
+  </si>
+  <si>
+    <t>Rat - 9/1</t>
+  </si>
+  <si>
+    <t>Rev - 7/1</t>
+  </si>
+  <si>
+    <t>Rat - 7/1</t>
+  </si>
+  <si>
     <t>Rev - 6/1</t>
   </si>
   <si>
     <t>Rat - 6/1</t>
   </si>
   <si>
-    <t>Rev - 5/1</t>
-  </si>
-  <si>
-    <t>Rat - 5/1</t>
+    <t>Weekly Sales (Ratings * 4)</t>
   </si>
 </sst>
 </file>
@@ -1434,13 +1443,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
@@ -1453,55 +1462,79 @@
       <c r="D1" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
-        <v>0</v>
+        <v>1279</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>5591</v>
       </c>
       <c r="C2">
+        <v>1279</v>
+      </c>
+      <c r="D2">
+        <v>5580</v>
+      </c>
+      <c r="E2">
         <v>1278</v>
       </c>
-      <c r="D2">
-        <v>5573</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2">
+        <v>5579</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
-        <v>0</v>
+        <v>442</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>729</v>
       </c>
       <c r="C3">
+        <v>428</v>
+      </c>
+      <c r="D3">
+        <v>704</v>
+      </c>
+      <c r="E3">
         <v>426</v>
       </c>
-      <c r="D3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
-        <v>0</v>
+        <v>2107</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>4829</v>
       </c>
       <c r="C4">
+        <v>2103</v>
+      </c>
+      <c r="D4">
+        <v>4823</v>
+      </c>
+      <c r="E4">
         <v>2102</v>
       </c>
-      <c r="D4">
-        <v>4819</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4">
+        <v>4823</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
-        <v>0</v>
+        <v>253</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>810</v>
       </c>
       <c r="C5">
         <v>251</v>
@@ -1509,139 +1542,199 @@
       <c r="D5">
         <v>808</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>251</v>
+      </c>
+      <c r="F5">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>241</v>
       </c>
       <c r="C6">
+        <v>146</v>
+      </c>
+      <c r="D6">
+        <v>218</v>
+      </c>
+      <c r="E6">
         <v>145</v>
       </c>
-      <c r="D6">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="F6">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
-        <v>0</v>
+        <v>715</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2080</v>
       </c>
       <c r="C7">
+        <v>707</v>
+      </c>
+      <c r="D7">
+        <v>2054</v>
+      </c>
+      <c r="E7">
         <v>705</v>
       </c>
-      <c r="D7">
-        <v>2051</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="F7">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
-        <v>0</v>
+        <v>454</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1474</v>
       </c>
       <c r="C8">
         <v>451</v>
       </c>
       <c r="D8">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>1462</v>
+      </c>
+      <c r="E8">
+        <v>451</v>
+      </c>
+      <c r="F8">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
-        <v>0</v>
+        <v>463</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>906</v>
       </c>
       <c r="C9">
+        <v>462</v>
+      </c>
+      <c r="D9">
+        <v>897</v>
+      </c>
+      <c r="E9">
         <v>461</v>
       </c>
-      <c r="D9">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="F9">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>421</v>
       </c>
       <c r="C10">
         <v>149</v>
       </c>
       <c r="D10">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>421</v>
+      </c>
+      <c r="E10">
+        <v>149</v>
+      </c>
+      <c r="F10">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
-        <v>0</v>
+        <v>532</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2486</v>
       </c>
       <c r="C11">
+        <v>528</v>
+      </c>
+      <c r="D11">
+        <v>2444</v>
+      </c>
+      <c r="E11">
         <v>526</v>
       </c>
-      <c r="D11">
-        <v>2430</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="F11">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
-        <v>0</v>
+        <v>533</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>1201</v>
       </c>
       <c r="C12">
         <v>532</v>
       </c>
       <c r="D12">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>1195</v>
+      </c>
+      <c r="E12">
+        <v>532</v>
+      </c>
+      <c r="F12">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
-        <v>0</v>
+        <v>389</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>1002</v>
       </c>
       <c r="C13">
         <v>389</v>
       </c>
       <c r="D13">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>998</v>
+      </c>
+      <c r="E13">
+        <v>389</v>
+      </c>
+      <c r="F13">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
-        <v>0</v>
+        <v>982</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>4121</v>
       </c>
       <c r="C14">
+        <v>982</v>
+      </c>
+      <c r="D14">
+        <v>4118</v>
+      </c>
+      <c r="E14">
         <v>981</v>
       </c>
-      <c r="D14">
-        <v>4114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="F14">
+        <v>4117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
-        <v>0</v>
+        <v>274</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>760</v>
       </c>
       <c r="C15">
         <v>274</v>
@@ -1649,13 +1742,19 @@
       <c r="D15">
         <v>759</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>274</v>
+      </c>
+      <c r="F15">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>790</v>
       </c>
       <c r="C16">
         <v>135</v>
@@ -1663,13 +1762,19 @@
       <c r="D16">
         <v>789</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>135</v>
+      </c>
+      <c r="F16">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="C17">
         <v>47</v>
@@ -1677,13 +1782,19 @@
       <c r="D17">
         <v>121</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>47</v>
+      </c>
+      <c r="F17">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>554</v>
       </c>
       <c r="C18">
         <v>183</v>
@@ -1691,13 +1802,19 @@
       <c r="D18">
         <v>554</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>183</v>
+      </c>
+      <c r="F18">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="C19">
         <v>120</v>
@@ -1705,33 +1822,51 @@
       <c r="D19">
         <v>192</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>120</v>
+      </c>
+      <c r="F19">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
-        <v>0</v>
+        <v>5750</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>21566</v>
       </c>
       <c r="C20">
-        <v>5717</v>
+        <v>5722</v>
       </c>
       <c r="D20">
-        <v>21431</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>21464</v>
+      </c>
+      <c r="E20">
+        <v>5718</v>
+      </c>
+      <c r="F20">
+        <v>21462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="C21">
         <v>42</v>
       </c>
       <c r="D21">
-        <v>158</v>
+        <v>159</v>
+      </c>
+      <c r="E21">
+        <v>42</v>
+      </c>
+      <c r="F21">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1741,13 +1876,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
@@ -1760,13 +1895,19 @@
       <c r="D1" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1175</v>
       </c>
       <c r="C2">
         <v>250</v>
@@ -1774,13 +1915,19 @@
       <c r="D2">
         <v>1175</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>250</v>
+      </c>
+      <c r="F2">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
-        <v>0</v>
+        <v>424</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2120</v>
       </c>
       <c r="C3">
         <v>424</v>
@@ -1788,13 +1935,19 @@
       <c r="D3">
         <v>2120</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>424</v>
+      </c>
+      <c r="F3">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
-        <v>0</v>
+        <v>714</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4096</v>
       </c>
       <c r="C4">
         <v>714</v>
@@ -1802,27 +1955,39 @@
       <c r="D4">
         <v>4096</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>714</v>
+      </c>
+      <c r="F4">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
-        <v>0</v>
+        <v>1197</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>7050</v>
       </c>
       <c r="C5">
+        <v>1197</v>
+      </c>
+      <c r="D5">
+        <v>7050</v>
+      </c>
+      <c r="E5">
         <v>1193</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>7011</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6">
-        <v>0</v>
+        <v>4541</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>27552</v>
       </c>
       <c r="C6">
         <v>4524</v>
@@ -1830,13 +1995,19 @@
       <c r="D6">
         <v>27372</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>4524</v>
+      </c>
+      <c r="F6">
+        <v>27372</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
-        <v>0</v>
+        <v>2232</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>14249</v>
       </c>
       <c r="C7">
         <v>2226</v>
@@ -1844,13 +2015,19 @@
       <c r="D7">
         <v>14173</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>2226</v>
+      </c>
+      <c r="F7">
+        <v>14173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
-        <v>0</v>
+        <v>2547</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>17045</v>
       </c>
       <c r="C8">
         <v>2547</v>
@@ -1858,13 +2035,19 @@
       <c r="D8">
         <v>17045</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>2547</v>
+      </c>
+      <c r="F8">
+        <v>17045</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
-        <v>0</v>
+        <v>1639</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>11051</v>
       </c>
       <c r="C9">
         <v>1613</v>
@@ -1872,27 +2055,39 @@
       <c r="D9">
         <v>10975</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>1613</v>
+      </c>
+      <c r="F9">
+        <v>10975</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
-        <v>0</v>
+        <v>1260</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>8079</v>
       </c>
       <c r="C10">
+        <v>1257</v>
+      </c>
+      <c r="D10">
+        <v>8052</v>
+      </c>
+      <c r="E10">
         <v>1255</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>8026</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:6">
       <c r="A11">
-        <v>0</v>
+        <v>585</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>4251</v>
       </c>
       <c r="C11">
         <v>585</v>
@@ -1900,13 +2095,19 @@
       <c r="D11">
         <v>4251</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>585</v>
+      </c>
+      <c r="F11">
+        <v>4251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
-        <v>0</v>
+        <v>4248</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>35364</v>
       </c>
       <c r="C12">
         <v>4248</v>
@@ -1914,41 +2115,59 @@
       <c r="D12">
         <v>35364</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>4248</v>
+      </c>
+      <c r="F12">
+        <v>35364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
-        <v>9</v>
+        <v>3048</v>
       </c>
       <c r="B13">
-        <v>48</v>
+        <v>23946</v>
       </c>
       <c r="C13">
-        <v>3039</v>
+        <v>3048</v>
       </c>
       <c r="D13">
-        <v>23898</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>23946</v>
+      </c>
+      <c r="E13">
+        <v>3048</v>
+      </c>
+      <c r="F13">
+        <v>23946</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
-        <v>0</v>
+        <v>4546</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>41791</v>
       </c>
       <c r="C14">
+        <v>4535</v>
+      </c>
+      <c r="D14">
+        <v>41608</v>
+      </c>
+      <c r="E14">
         <v>4527</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>41532</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6">
       <c r="A15">
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>2957</v>
       </c>
       <c r="C15">
         <v>192</v>
@@ -1956,13 +2175,19 @@
       <c r="D15">
         <v>2923</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>192</v>
+      </c>
+      <c r="F15">
+        <v>2923</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -1970,13 +2195,19 @@
       <c r="D16">
         <v>191</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -1984,13 +2215,19 @@
       <c r="D17">
         <v>191</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>2329</v>
       </c>
       <c r="C18">
         <v>121</v>
@@ -1998,27 +2235,39 @@
       <c r="D18">
         <v>2329</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>121</v>
+      </c>
+      <c r="F18">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>909</v>
       </c>
       <c r="C19">
         <v>40</v>
       </c>
       <c r="D19">
+        <v>909</v>
+      </c>
+      <c r="E19">
+        <v>40</v>
+      </c>
+      <c r="F19">
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:6">
       <c r="A20">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="C20">
         <v>21</v>
@@ -2026,13 +2275,19 @@
       <c r="D20">
         <v>120</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>21</v>
+      </c>
+      <c r="F20">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="C21">
         <v>50</v>
@@ -2040,13 +2295,19 @@
       <c r="D21">
         <v>446</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="F21">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
-        <v>0</v>
+        <v>1188</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>10993</v>
       </c>
       <c r="C22">
         <v>1188</v>
@@ -2054,13 +2315,19 @@
       <c r="D22">
         <v>10993</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>1188</v>
+      </c>
+      <c r="F22">
+        <v>10993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
-        <v>0</v>
+        <v>496</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>5134</v>
       </c>
       <c r="C23">
         <v>489</v>
@@ -2068,27 +2335,39 @@
       <c r="D23">
         <v>5056</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>489</v>
+      </c>
+      <c r="F23">
+        <v>5056</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
-        <v>0</v>
+        <v>1517</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>9759</v>
       </c>
       <c r="C24">
+        <v>1516</v>
+      </c>
+      <c r="D24">
+        <v>9755</v>
+      </c>
+      <c r="E24">
         <v>1513</v>
       </c>
-      <c r="D24">
+      <c r="F24">
         <v>9699</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:6">
       <c r="A25">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1022</v>
       </c>
       <c r="C25">
         <v>116</v>
@@ -2096,13 +2375,19 @@
       <c r="D25">
         <v>1022</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>116</v>
+      </c>
+      <c r="F25">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="C26">
         <v>18</v>
@@ -2110,27 +2395,39 @@
       <c r="D26">
         <v>139</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>18</v>
+      </c>
+      <c r="F26">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>506</v>
       </c>
       <c r="C27">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D27">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>506</v>
+      </c>
+      <c r="E27">
+        <v>80</v>
+      </c>
+      <c r="F27">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="C28">
         <v>14</v>
@@ -2138,27 +2435,39 @@
       <c r="D28">
         <v>194</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>14</v>
+      </c>
+      <c r="F28">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1213</v>
       </c>
       <c r="C29">
         <v>305</v>
       </c>
       <c r="D29">
+        <v>1213</v>
+      </c>
+      <c r="E29">
+        <v>305</v>
+      </c>
+      <c r="F29">
         <v>1214</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:6">
       <c r="A30">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="C30">
         <v>34</v>
@@ -2166,27 +2475,39 @@
       <c r="D30">
         <v>230</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>34</v>
+      </c>
+      <c r="F30">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>306</v>
       </c>
       <c r="C31">
+        <v>59</v>
+      </c>
+      <c r="D31">
+        <v>306</v>
+      </c>
+      <c r="E31">
         <v>58</v>
       </c>
-      <c r="D31">
+      <c r="F31">
         <v>303</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:6">
       <c r="A32">
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>886</v>
       </c>
       <c r="C32">
         <v>157</v>
@@ -2194,18 +2515,30 @@
       <c r="D32">
         <v>886</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>157</v>
+      </c>
+      <c r="F32">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>562</v>
       </c>
       <c r="C33">
         <v>68</v>
       </c>
       <c r="D33">
+        <v>560</v>
+      </c>
+      <c r="E33">
+        <v>68</v>
+      </c>
+      <c r="F33">
         <v>560</v>
       </c>
     </row>
@@ -2216,782 +2549,1324 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>5591</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>5579</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>729</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>4829</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>4823</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>810</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>241</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>2080</v>
+      </c>
+      <c r="E7">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>1474</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9">
+        <v>906</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10">
+        <v>421</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>2486</v>
+      </c>
+      <c r="E11">
+        <v>42</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12">
+        <v>1201</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <v>1002</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14">
+        <v>4121</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>4117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15">
+        <v>760</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16">
+        <v>790</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <v>122</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
         <v>121</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1278</v>
-      </c>
-      <c r="D2">
-        <v>5573</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>426</v>
-      </c>
-      <c r="D3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2102</v>
-      </c>
-      <c r="D4">
-        <v>4819</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>251</v>
-      </c>
-      <c r="D5">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>145</v>
-      </c>
-      <c r="D6">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>705</v>
-      </c>
-      <c r="D7">
-        <v>2051</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>451</v>
-      </c>
-      <c r="D8">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>461</v>
-      </c>
-      <c r="D9">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>149</v>
-      </c>
-      <c r="D10">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>526</v>
-      </c>
-      <c r="D11">
-        <v>2430</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>532</v>
-      </c>
-      <c r="D12">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>389</v>
-      </c>
-      <c r="D13">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>981</v>
-      </c>
-      <c r="D14">
-        <v>4114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>274</v>
-      </c>
-      <c r="D15">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>135</v>
-      </c>
-      <c r="D16">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>47</v>
-      </c>
-      <c r="D17">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>183</v>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D18">
         <v>554</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>120</v>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D19">
         <v>192</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>6</v>
-      </c>
-      <c r="C20">
-        <v>5717</v>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D20">
-        <v>21431</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>42</v>
+        <v>21566</v>
+      </c>
+      <c r="E20">
+        <v>102</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>21462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="D21">
-        <v>158</v>
+        <v>159</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C21" r:id="rId20"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>250</v>
+      <c r="G1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="D2">
         <v>1175</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>424</v>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="D3">
         <v>2120</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>714</v>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="D4">
         <v>4096</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1193</v>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D5">
+        <v>7050</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>39</v>
+      </c>
+      <c r="G5">
         <v>7011</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>4524</v>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="D6">
+        <v>27552</v>
+      </c>
+      <c r="E6">
+        <v>180</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>27372</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>2226</v>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D7">
+        <v>14249</v>
+      </c>
+      <c r="E7">
+        <v>76</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>14173</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>2547</v>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="D8">
         <v>17045</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1613</v>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>17045</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D9">
+        <v>11051</v>
+      </c>
+      <c r="E9">
+        <v>76</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>10975</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1255</v>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D10">
+        <v>8079</v>
+      </c>
+      <c r="E10">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <v>26</v>
+      </c>
+      <c r="G10">
         <v>8026</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>585</v>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="D11">
         <v>4251</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>4248</v>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>4251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D12">
         <v>35364</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>48</v>
-      </c>
-      <c r="C13">
-        <v>3039</v>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>35364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="D13">
-        <v>23898</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>4527</v>
+        <v>23946</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>23946</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D14">
+        <v>41791</v>
+      </c>
+      <c r="E14">
+        <v>183</v>
+      </c>
+      <c r="F14">
+        <v>76</v>
+      </c>
+      <c r="G14">
         <v>41532</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>192</v>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="D15">
+        <v>2957</v>
+      </c>
+      <c r="E15">
+        <v>34</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>2923</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="D16">
+        <v>196</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>10</v>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D17">
+        <v>196</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
         <v>191</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>121</v>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="D18">
         <v>2329</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>40</v>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="D19">
+        <v>909</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+      <c r="G19">
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>21</v>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="D20">
         <v>120</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>50</v>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="D21">
         <v>446</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>1188</v>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="D22">
         <v>10993</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>489</v>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>10993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="D23">
+        <v>5134</v>
+      </c>
+      <c r="E23">
+        <v>78</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
         <v>5056</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>1513</v>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="D24">
+        <v>9759</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>56</v>
+      </c>
+      <c r="G24">
         <v>9699</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>116</v>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D25">
         <v>1022</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>18</v>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="D26">
+        <v>147</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27">
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27">
+        <v>506</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
         <v>1</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>79</v>
-      </c>
-      <c r="D27">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>14</v>
+      <c r="G27">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="D28">
         <v>194</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29">
-        <v>0</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>305</v>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D29">
+        <v>1213</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>-1</v>
+      </c>
+      <c r="G29">
         <v>1214</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
-        <v>0</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>34</v>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="D30">
         <v>230</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31">
-        <v>0</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>58</v>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="D31">
+        <v>306</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31">
         <v>303</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32">
-        <v>0</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>157</v>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="D32">
         <v>886</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33">
-        <v>0</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>68</v>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="D33">
+        <v>562</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
         <v>560</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C21" r:id="rId20"/>
+    <hyperlink ref="C22" r:id="rId21"/>
+    <hyperlink ref="C23" r:id="rId22"/>
+    <hyperlink ref="C24" r:id="rId23"/>
+    <hyperlink ref="C25" r:id="rId24"/>
+    <hyperlink ref="C26" r:id="rId25"/>
+    <hyperlink ref="C27" r:id="rId26"/>
+    <hyperlink ref="C28" r:id="rId27"/>
+    <hyperlink ref="C29" r:id="rId28"/>
+    <hyperlink ref="C30" r:id="rId29"/>
+    <hyperlink ref="C31" r:id="rId30"/>
+    <hyperlink ref="C32" r:id="rId31"/>
+    <hyperlink ref="C33" r:id="rId32"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>